<commit_message>
Updated data file with periods info.
</commit_message>
<xml_diff>
--- a/Parameters/DataPeriods.xlsx
+++ b/Parameters/DataPeriods.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DES.LM.UserFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dim-Dim\MyData\Common Work Place\Projects\DES.LM.Reports\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E060972A-614E-4C3B-AC7A-59905E65F39D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F0B8EA-FCA2-402C-8F55-AE1B254077A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-12045" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Periods" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" calcCompleted="0" calcOnSave="0"/>
+  <calcPr calcId="162913" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
   <si>
     <t>StartMonth</t>
   </si>
@@ -33,48 +33,18 @@
     <t>EndMonth</t>
   </si>
   <si>
-    <t>PeriodName</t>
-  </si>
-  <si>
     <t>01. С начала года до текущего месяца</t>
   </si>
   <si>
     <t>03. Текущий месяц</t>
   </si>
   <si>
-    <t>04. Предыдущий месяц</t>
-  </si>
-  <si>
-    <t>02. С начала года до предыдущего месяца</t>
-  </si>
-  <si>
-    <t>05. Первый квартал</t>
-  </si>
-  <si>
-    <t>06. Второй квартал</t>
-  </si>
-  <si>
-    <t>07. Третий квартал</t>
-  </si>
-  <si>
-    <t>08. Четвёртый квартал</t>
-  </si>
-  <si>
-    <t>08. Первое полугодие</t>
-  </si>
-  <si>
-    <t>09. Второе полугодие</t>
-  </si>
-  <si>
     <t>this</t>
   </si>
   <si>
     <t>01</t>
   </si>
   <si>
-    <t>02</t>
-  </si>
-  <si>
     <t>03</t>
   </si>
   <si>
@@ -102,7 +72,34 @@
     <t>11. Весь год (12 месяцев)</t>
   </si>
   <si>
-    <t>10. 1й, 2й и 3й кварталы</t>
+    <t>DataPeriodName</t>
+  </si>
+  <si>
+    <t>04. Предыдущий месяц (но не ранее января)</t>
+  </si>
+  <si>
+    <t>02. С начала года до предыдущего месяца (но не ранее января)</t>
+  </si>
+  <si>
+    <t>05. Первый квартал (январь - март)</t>
+  </si>
+  <si>
+    <t>06. Второй квартал (апрель - июнь)</t>
+  </si>
+  <si>
+    <t>08. Четвёртый квартал (октябрь - декабрь)</t>
+  </si>
+  <si>
+    <t>08. Первое полугодие (январь - июнь)</t>
+  </si>
+  <si>
+    <t>09. Второе полугодие (июль - декабрь)</t>
+  </si>
+  <si>
+    <t>10. 1й, 2й и 3й кварталы (январь - сентябрь)</t>
+  </si>
+  <si>
+    <t>07. Третий квартал (июль - сентябрь)</t>
   </si>
 </sst>
 </file>
@@ -440,18 +437,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.28515625" customWidth="1"/>
+    <col min="1" max="1" width="60.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -462,134 +461,134 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="C8" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>